<commit_message>
Add iostream and a protected keyword
</commit_message>
<xml_diff>
--- a/doc/Inspector-Keybindings.xlsx
+++ b/doc/Inspector-Keybindings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="23715" windowHeight="9525"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Picviz Inspector Default Keybindings</t>
   </si>
@@ -286,30 +286,6 @@
     <t>ALT + U</t>
   </si>
   <si>
-    <t>Add lines</t>
-  </si>
-  <si>
-    <t>Remove lines</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Add selected lines to</t>
-  </si>
-  <si>
-    <t>Remove selected lines from</t>
-  </si>
-  <si>
-    <t>the active layer***</t>
-  </si>
-  <si>
-    <t>the active layer*** of the layer stack</t>
-  </si>
-  <si>
     <t>*** If the active layer is linked to other layers, the operation applies to all linked layers</t>
   </si>
   <si>
@@ -323,9 +299,6 @@
   </si>
   <si>
     <t>Activate / Deactivate</t>
-  </si>
-  <si>
-    <t>anti-aliasing</t>
   </si>
   <si>
     <t>Initial position</t>
@@ -382,13 +355,16 @@
   </si>
   <si>
     <t xml:space="preserve">Select all lines but </t>
+  </si>
+  <si>
+    <t>anti-aliasing (dangerous)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,14 +491,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,6 +506,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -577,7 +558,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -651,6 +632,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -685,6 +667,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -860,14 +843,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
@@ -878,13 +861,13 @@
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -897,24 +880,24 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" ht="23.25">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -927,23 +910,23 @@
       <c r="D4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>91</v>
+      <c r="E4" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -963,21 +946,21 @@
         <v>62</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75">
-      <c r="A6" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
       <c r="F6" s="3" t="s">
@@ -985,21 +968,21 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="7" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
@@ -1008,19 +991,19 @@
         <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -1038,7 +1021,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="C9" s="3" t="s">
         <v>14</v>
@@ -1055,7 +1038,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -1073,7 +1056,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -1095,12 +1078,12 @@
       <c r="H11" s="7"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="F12" s="3" t="s">
@@ -1109,7 +1092,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>67</v>
       </c>
@@ -1129,7 +1112,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="3" t="s">
@@ -1143,7 +1126,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1163,7 +1146,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
@@ -1179,7 +1162,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>65</v>
       </c>
@@ -1201,7 +1184,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>66</v>
       </c>
@@ -1221,7 +1204,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="7"/>
       <c r="C19" s="3" t="s">
@@ -1235,12 +1218,12 @@
       <c r="H19" s="7"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="4"/>
       <c r="E20" s="7" t="s">
         <v>71</v>
@@ -1251,7 +1234,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>47</v>
       </c>
@@ -1270,7 +1253,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1287,7 +1270,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1311,7 +1294,7 @@
       <c r="L23" s="7"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
@@ -1328,12 +1311,12 @@
       <c r="H24" s="7"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75">
-      <c r="A25" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="4"/>
       <c r="E25" s="7"/>
       <c r="F25" s="3" t="s">
@@ -1343,67 +1326,51 @@
       <c r="H25" s="7"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="7"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="C27" s="14" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="F27" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="7"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
-      <c r="D28" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>79</v>
-      </c>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="7"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="7"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
@@ -1416,7 +1383,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
@@ -1429,9 +1396,9 @@
       <c r="H31" s="7"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="3"/>
@@ -1459,24 +1426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>